<commit_message>
Luma project commit new
</commit_message>
<xml_diff>
--- a/Luma_testdata.xlsx
+++ b/Luma_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_testing-files\Automation_project1-main\Luma-Prj1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B044D92E-7374-4C8A-A643-527A934C6A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334019E0-7664-46E4-9518-84DFA45DAA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>Create New Customer Account</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Tees</t>
+  </si>
+  <si>
+    <t>Raghunew@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -606,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>